<commit_message>
Letter Combinations of a Phone Number done
</commit_message>
<xml_diff>
--- a/思考.xlsx
+++ b/思考.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5d28c77152a8a29/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="358" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{040363EF-2147-4168-A814-F640E72A68D0}"/>
+  <xr:revisionPtr revIDLastSave="383" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF33E9FE-9226-46C1-9881-751F53AF17BF}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,9 +300,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -670,10 +667,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="E6:T64"/>
+  <dimension ref="E6:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="F67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -923,14 +920,6 @@
       </c>
     </row>
     <row r="23" spans="5:20" x14ac:dyDescent="0.3">
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
       <c r="Q23" s="1" t="s">
         <v>9</v>
       </c>
@@ -939,14 +928,6 @@
       </c>
     </row>
     <row r="24" spans="5:20" x14ac:dyDescent="0.3">
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
       <c r="Q24" s="1" t="s">
         <v>10</v>
       </c>
@@ -954,25 +935,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="5:20" x14ac:dyDescent="0.3">
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-    </row>
     <row r="26" spans="5:20" x14ac:dyDescent="0.3">
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
       <c r="Q26" s="1" t="s">
         <v>11</v>
       </c>
@@ -980,180 +943,118 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="5:20" x14ac:dyDescent="0.3">
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-    </row>
-    <row r="48" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-    </row>
     <row r="49" spans="5:13" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F49" s="8">
-        <v>1</v>
-      </c>
-      <c r="G49" s="8">
-        <v>2</v>
-      </c>
-      <c r="H49" s="8">
-        <v>3</v>
-      </c>
-      <c r="I49" s="8">
-        <v>4</v>
-      </c>
-      <c r="J49" s="8">
-        <v>5</v>
-      </c>
-      <c r="K49" s="8">
-        <v>6</v>
-      </c>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1">
+        <v>2</v>
+      </c>
+      <c r="H49" s="1">
+        <v>3</v>
+      </c>
+      <c r="I49" s="1">
+        <v>4</v>
+      </c>
+      <c r="J49" s="1">
+        <v>5</v>
+      </c>
+      <c r="K49" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="50" spans="5:13" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E50" s="1">
         <v>1</v>
       </c>
-      <c r="F50" s="9"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" spans="5:13" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E51" s="1">
         <v>2</v>
       </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
+      <c r="F51" s="10"/>
     </row>
     <row r="52" spans="5:13" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E52" s="1">
         <v>3</v>
       </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="14"/>
     </row>
     <row r="53" spans="5:13" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E53" s="1">
         <v>4</v>
       </c>
-      <c r="F53" s="9"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="10"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="9"/>
     </row>
     <row r="54" spans="5:13" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E54" s="1">
         <v>5</v>
       </c>
-      <c r="F54" s="13"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="14"/>
     </row>
     <row r="55" spans="5:13" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E55" s="1">
         <v>6</v>
       </c>
-      <c r="F55" s="9"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="8"/>
-      <c r="M55" s="8"/>
-    </row>
-    <row r="56" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-    </row>
-    <row r="57" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="9"/>
     </row>
     <row r="58" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="F58" s="8">
-        <v>1</v>
-      </c>
-      <c r="G58" s="8">
-        <v>2</v>
-      </c>
-      <c r="H58" s="8">
-        <v>3</v>
-      </c>
-      <c r="I58" s="8">
-        <v>4</v>
-      </c>
-      <c r="J58" s="8">
-        <v>5</v>
-      </c>
-      <c r="K58" s="8">
-        <v>6</v>
-      </c>
-      <c r="L58" s="8"/>
-      <c r="M58" s="8"/>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1">
+        <v>2</v>
+      </c>
+      <c r="H58" s="1">
+        <v>3</v>
+      </c>
+      <c r="I58" s="1">
+        <v>4</v>
+      </c>
+      <c r="J58" s="1">
+        <v>5</v>
+      </c>
+      <c r="K58" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="59" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E59" s="1">
         <v>1</v>
       </c>
-      <c r="F59" s="16">
-        <v>1</v>
-      </c>
-      <c r="G59" s="16">
-        <v>1</v>
-      </c>
-      <c r="H59" s="16">
-        <v>1</v>
-      </c>
-      <c r="I59" s="16">
-        <v>1</v>
-      </c>
-      <c r="J59" s="16">
-        <v>1</v>
-      </c>
-      <c r="K59" s="16">
-        <v>1</v>
-      </c>
-      <c r="L59" s="8"/>
-      <c r="M59" s="8">
+      <c r="F59" s="15">
+        <v>1</v>
+      </c>
+      <c r="G59" s="15">
+        <v>1</v>
+      </c>
+      <c r="H59" s="15">
+        <v>1</v>
+      </c>
+      <c r="I59" s="15">
+        <v>1</v>
+      </c>
+      <c r="J59" s="15">
+        <v>1</v>
+      </c>
+      <c r="K59" s="15">
+        <v>1</v>
+      </c>
+      <c r="M59" s="1">
         <v>6</v>
       </c>
     </row>
@@ -1161,26 +1062,25 @@
       <c r="E60" s="1">
         <v>2</v>
       </c>
-      <c r="F60" s="16">
-        <v>2</v>
-      </c>
-      <c r="G60" s="16">
-        <v>0</v>
-      </c>
-      <c r="H60" s="16">
-        <v>2</v>
-      </c>
-      <c r="I60" s="16">
-        <v>2</v>
-      </c>
-      <c r="J60" s="16">
-        <v>2</v>
-      </c>
-      <c r="K60" s="16">
-        <v>2</v>
-      </c>
-      <c r="L60" s="8"/>
-      <c r="M60" s="8">
+      <c r="F60" s="15">
+        <v>2</v>
+      </c>
+      <c r="G60" s="15">
+        <v>0</v>
+      </c>
+      <c r="H60" s="15">
+        <v>2</v>
+      </c>
+      <c r="I60" s="15">
+        <v>2</v>
+      </c>
+      <c r="J60" s="15">
+        <v>2</v>
+      </c>
+      <c r="K60" s="15">
+        <v>2</v>
+      </c>
+      <c r="M60" s="1">
         <v>8</v>
       </c>
     </row>
@@ -1188,26 +1088,25 @@
       <c r="E61" s="1">
         <v>3</v>
       </c>
-      <c r="F61" s="16">
-        <v>0</v>
-      </c>
-      <c r="G61" s="16">
-        <v>0</v>
-      </c>
-      <c r="H61" s="16">
-        <v>3</v>
-      </c>
-      <c r="I61" s="16">
-        <v>3</v>
-      </c>
-      <c r="J61" s="16">
-        <v>0</v>
-      </c>
-      <c r="K61" s="16">
-        <v>3</v>
-      </c>
-      <c r="L61" s="8"/>
-      <c r="M61" s="8">
+      <c r="F61" s="15">
+        <v>0</v>
+      </c>
+      <c r="G61" s="15">
+        <v>0</v>
+      </c>
+      <c r="H61" s="15">
+        <v>3</v>
+      </c>
+      <c r="I61" s="15">
+        <v>3</v>
+      </c>
+      <c r="J61" s="15">
+        <v>0</v>
+      </c>
+      <c r="K61" s="15">
+        <v>3</v>
+      </c>
+      <c r="M61" s="1">
         <v>6</v>
       </c>
     </row>
@@ -1215,22 +1114,22 @@
       <c r="E62" s="1">
         <v>4</v>
       </c>
-      <c r="F62" s="16">
-        <v>0</v>
-      </c>
-      <c r="G62" s="16">
-        <v>0</v>
-      </c>
-      <c r="H62" s="16">
-        <v>4</v>
-      </c>
-      <c r="I62" s="16">
-        <v>4</v>
-      </c>
-      <c r="J62" s="16">
-        <v>0</v>
-      </c>
-      <c r="K62" s="16">
+      <c r="F62" s="15">
+        <v>0</v>
+      </c>
+      <c r="G62" s="15">
+        <v>0</v>
+      </c>
+      <c r="H62" s="15">
+        <v>4</v>
+      </c>
+      <c r="I62" s="15">
+        <v>4</v>
+      </c>
+      <c r="J62" s="15">
+        <v>0</v>
+      </c>
+      <c r="K62" s="15">
         <v>0</v>
       </c>
       <c r="M62" s="1">
@@ -1241,22 +1140,22 @@
       <c r="E63" s="1">
         <v>5</v>
       </c>
-      <c r="F63" s="16">
-        <v>0</v>
-      </c>
-      <c r="G63" s="16">
-        <v>0</v>
-      </c>
-      <c r="H63" s="16">
-        <v>5</v>
-      </c>
-      <c r="I63" s="16">
-        <v>5</v>
-      </c>
-      <c r="J63" s="16">
-        <v>0</v>
-      </c>
-      <c r="K63" s="16">
+      <c r="F63" s="15">
+        <v>0</v>
+      </c>
+      <c r="G63" s="15">
+        <v>0</v>
+      </c>
+      <c r="H63" s="15">
+        <v>5</v>
+      </c>
+      <c r="I63" s="15">
+        <v>5</v>
+      </c>
+      <c r="J63" s="15">
+        <v>0</v>
+      </c>
+      <c r="K63" s="15">
         <v>0</v>
       </c>
       <c r="M63" s="1">
@@ -1267,26 +1166,86 @@
       <c r="E64" s="1">
         <v>6</v>
       </c>
-      <c r="F64" s="16">
-        <v>0</v>
-      </c>
-      <c r="G64" s="16">
-        <v>0</v>
-      </c>
-      <c r="H64" s="16">
-        <v>0</v>
-      </c>
-      <c r="I64" s="16">
-        <v>6</v>
-      </c>
-      <c r="J64" s="16">
-        <v>0</v>
-      </c>
-      <c r="K64" s="16">
+      <c r="F64" s="15">
+        <v>0</v>
+      </c>
+      <c r="G64" s="15">
+        <v>0</v>
+      </c>
+      <c r="H64" s="15">
+        <v>0</v>
+      </c>
+      <c r="I64" s="15">
+        <v>6</v>
+      </c>
+      <c r="J64" s="15">
+        <v>0</v>
+      </c>
+      <c r="K64" s="15">
         <v>0</v>
       </c>
       <c r="M64" s="1">
         <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H72" s="1">
+        <v>1</v>
+      </c>
+      <c r="I72" s="1">
+        <v>2</v>
+      </c>
+      <c r="J72" s="1">
+        <v>3</v>
+      </c>
+      <c r="K72" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="J73" s="1">
+        <v>4</v>
+      </c>
+      <c r="K73" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="I75" s="1">
+        <v>3</v>
+      </c>
+      <c r="J75" s="1">
+        <v>2</v>
+      </c>
+      <c r="K75" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="J76" s="1">
+        <v>4</v>
+      </c>
+      <c r="K76" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="I78" s="1">
+        <v>4</v>
+      </c>
+      <c r="J78" s="1">
+        <v>2</v>
+      </c>
+      <c r="K78" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="J79" s="1">
+        <v>3</v>
+      </c>
+      <c r="K79" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maximum XOR of Two Numbers in an Array not done(See Solution)
</commit_message>
<xml_diff>
--- a/思考.xlsx
+++ b/思考.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5d28c77152a8a29/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="383" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF33E9FE-9226-46C1-9881-751F53AF17BF}"/>
+  <xr:revisionPtr revIDLastSave="464" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E7FF7F6-78C8-4016-8BB2-20170E58E2C1}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -667,15 +668,16 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="E6:T79"/>
+  <dimension ref="E6:T97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72"/>
+    <sheetView tabSelected="1" topLeftCell="F82" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N87" sqref="N87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="9" style="1"/>
+    <col min="1" max="8" width="9" style="1"/>
+    <col min="9" max="9" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
@@ -1248,7 +1250,232 @@
         <v>2</v>
       </c>
     </row>
+    <row r="83" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="N83" s="1">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H85" s="1">
+        <v>14</v>
+      </c>
+      <c r="I85" s="1" t="str">
+        <f t="shared" ref="I85:I96" si="0">DEC2BIN(H85,8)</f>
+        <v>00001110</v>
+      </c>
+      <c r="L85" s="1">
+        <v>14</v>
+      </c>
+      <c r="M85" s="1" t="str">
+        <f t="shared" ref="M85:M96" si="1">DEC2BIN(L85,8)</f>
+        <v>00001110</v>
+      </c>
+      <c r="N85" s="1">
+        <f>_xlfn.BITXOR(L85,$N83)</f>
+        <v>113</v>
+      </c>
+      <c r="P85" s="1" t="str">
+        <f>DEC2BIN(127,8)</f>
+        <v>01111111</v>
+      </c>
+      <c r="Q85" s="1" t="str">
+        <f>DEC2BIN(28,8)</f>
+        <v>00011100</v>
+      </c>
+    </row>
+    <row r="86" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H86" s="1">
+        <v>70</v>
+      </c>
+      <c r="I86" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>01000110</v>
+      </c>
+      <c r="L86" s="1">
+        <v>36</v>
+      </c>
+      <c r="M86" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00100100</v>
+      </c>
+      <c r="N86" s="1">
+        <f>_xlfn.BITXOR(L86,$N83)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="87" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H87" s="1">
+        <v>53</v>
+      </c>
+      <c r="I87" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>00110101</v>
+      </c>
+      <c r="L87" s="1">
+        <v>49</v>
+      </c>
+      <c r="M87" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00110001</v>
+      </c>
+    </row>
+    <row r="88" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H88" s="1">
+        <v>83</v>
+      </c>
+      <c r="I88" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>01010011</v>
+      </c>
+      <c r="L88" s="1">
+        <v>51</v>
+      </c>
+      <c r="M88" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00110011</v>
+      </c>
+    </row>
+    <row r="89" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H89" s="1">
+        <v>49</v>
+      </c>
+      <c r="I89" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>00110001</v>
+      </c>
+      <c r="L89" s="1">
+        <v>53</v>
+      </c>
+      <c r="M89" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00110101</v>
+      </c>
+    </row>
+    <row r="90" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H90" s="1">
+        <v>91</v>
+      </c>
+      <c r="I90" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>01011011</v>
+      </c>
+      <c r="L90" s="1">
+        <v>66</v>
+      </c>
+      <c r="M90" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>01000010</v>
+      </c>
+    </row>
+    <row r="91" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H91" s="1">
+        <v>36</v>
+      </c>
+      <c r="I91" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>00100100</v>
+      </c>
+      <c r="L91" s="1">
+        <v>70</v>
+      </c>
+      <c r="M91" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>01000110</v>
+      </c>
+    </row>
+    <row r="92" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H92" s="1">
+        <v>80</v>
+      </c>
+      <c r="I92" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>01010000</v>
+      </c>
+      <c r="L92" s="1">
+        <v>70</v>
+      </c>
+      <c r="M92" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>01000110</v>
+      </c>
+    </row>
+    <row r="93" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H93" s="1">
+        <v>92</v>
+      </c>
+      <c r="I93" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>01011100</v>
+      </c>
+      <c r="L93" s="1">
+        <v>80</v>
+      </c>
+      <c r="M93" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>01010000</v>
+      </c>
+    </row>
+    <row r="94" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H94" s="1">
+        <v>51</v>
+      </c>
+      <c r="I94" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>00110011</v>
+      </c>
+      <c r="L94" s="1">
+        <v>83</v>
+      </c>
+      <c r="M94" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>01010011</v>
+      </c>
+    </row>
+    <row r="95" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H95" s="1">
+        <v>66</v>
+      </c>
+      <c r="I95" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>01000010</v>
+      </c>
+      <c r="L95" s="1">
+        <v>91</v>
+      </c>
+      <c r="M95" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>01011011</v>
+      </c>
+    </row>
+    <row r="96" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H96" s="1">
+        <v>70</v>
+      </c>
+      <c r="I96" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>01000110</v>
+      </c>
+      <c r="L96" s="1">
+        <v>92</v>
+      </c>
+      <c r="M96" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>01011100</v>
+      </c>
+      <c r="P96" s="1">
+        <v>100011</v>
+      </c>
+    </row>
+    <row r="97" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P97" s="1">
+        <f>_xlfn.BITXOR(92,127)</f>
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L85:M96">
+    <sortCondition ref="L85:L96"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Word Search II not done(See Solution)
</commit_message>
<xml_diff>
--- a/思考.xlsx
+++ b/思考.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5d28c77152a8a29/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="464" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E7FF7F6-78C8-4016-8BB2-20170E58E2C1}"/>
+  <xr:revisionPtr revIDLastSave="500" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B309A734-51E5-4403-9242-8992F47F0467}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>L</t>
   </si>
@@ -79,6 +78,106 @@
   </si>
   <si>
     <t>res</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">n </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -668,10 +767,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="E6:T97"/>
+  <dimension ref="E6:T123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F82" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N87" sqref="N87"/>
+    <sheetView tabSelected="1" topLeftCell="H115" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1466,10 +1565,130 @@
         <v>100011</v>
       </c>
     </row>
-    <row r="97" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="10:16" x14ac:dyDescent="0.3">
       <c r="P97" s="1">
         <f>_xlfn.BITXOR(92,127)</f>
         <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L111" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M112" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="J113" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="J114" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="J118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="J119" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="120" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="J120" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L120" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="121" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="J121" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L121" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="123" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I123" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J123" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Palindrome Pairs not done(See Solutions)
</commit_message>
<xml_diff>
--- a/思考.xlsx
+++ b/思考.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5d28c77152a8a29/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="500" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B309A734-51E5-4403-9242-8992F47F0467}"/>
+  <xr:revisionPtr revIDLastSave="680" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{781EE6C2-CEC4-4400-9E09-03CA5435F3B1}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="51">
   <si>
     <t>L</t>
   </si>
@@ -178,6 +178,62 @@
   </si>
   <si>
     <t>o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>abcd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dcba</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sssll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ac</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -379,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -424,6 +480,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +826,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="E6:T123"/>
+  <dimension ref="E6:W158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H115" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J119" sqref="J119"/>
+    <sheetView tabSelected="1" topLeftCell="I148" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="V154" sqref="V154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -778,7 +837,9 @@
     <col min="1" max="8" width="9" style="1"/>
     <col min="9" max="9" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="1"/>
+    <col min="11" max="12" width="9" style="1"/>
+    <col min="13" max="13" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="5:13" x14ac:dyDescent="0.3">
@@ -1599,7 +1660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J113" s="1" t="s">
         <v>13</v>
       </c>
@@ -1613,7 +1674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J114" s="1" t="s">
         <v>13</v>
       </c>
@@ -1627,7 +1688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J118" s="1" t="s">
         <v>12</v>
       </c>
@@ -1641,7 +1702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J119" s="1" t="s">
         <v>26</v>
       </c>
@@ -1655,7 +1716,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J120" s="1" t="s">
         <v>28</v>
       </c>
@@ -1669,7 +1730,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="121" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J121" s="1" t="s">
         <v>28</v>
       </c>
@@ -1683,18 +1744,375 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="123" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I123" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J123" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="9:23" x14ac:dyDescent="0.3">
+      <c r="S125" s="1">
+        <v>0</v>
+      </c>
+      <c r="T125" s="1">
+        <v>1</v>
+      </c>
+      <c r="U125" s="1">
+        <v>2</v>
+      </c>
+      <c r="V125" s="1">
+        <v>3</v>
+      </c>
+      <c r="W125" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="9:23" x14ac:dyDescent="0.3">
+      <c r="S126" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T126" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U126" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V126" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W126" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="127" spans="9:23" x14ac:dyDescent="0.3">
+      <c r="S127" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U127" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W127" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="128" spans="9:23" x14ac:dyDescent="0.3">
+      <c r="S128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T128" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U128" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W128" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="S129" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W129" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="130" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K130" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L130" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N130" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O130" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W130" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="133" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="U133" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="V133" s="16"/>
+    </row>
+    <row r="134" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K134" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L134" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M134" s="1" t="str">
+        <f>_xlfn.CONCAT(L134,K134)</f>
+        <v>abcdlls</v>
+      </c>
+      <c r="T134" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U134" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V134" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W134" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="135" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K135" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M135" s="1" t="str">
+        <f t="shared" ref="M135:M144" si="2">_xlfn.CONCAT(L135,K135)</f>
+        <v>dcballs</v>
+      </c>
+      <c r="T135" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V135" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W135" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K136" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L136" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U136" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V136" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W136" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="137" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K137" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M137" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>slls</v>
+      </c>
+      <c r="T137" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U137" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W137" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="138" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K138" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M138" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ssslllls</v>
+      </c>
+      <c r="W138" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="139" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="M139" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K140" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M140" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>abcds</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q140" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R140" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="141" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K141" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M141" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dcbas</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q141" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R141" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="142" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K142" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L142" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M142" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>llss</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q142" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R142" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="143" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K143" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q143" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R143" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="144" spans="11:23" x14ac:dyDescent="0.3">
+      <c r="K144" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L144" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M144" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ssslls</v>
+      </c>
+    </row>
+    <row r="152" spans="11:21" x14ac:dyDescent="0.3">
+      <c r="S152" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="153" spans="11:21" x14ac:dyDescent="0.3">
+      <c r="K153" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R153" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T153" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U153" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="154" spans="11:21" x14ac:dyDescent="0.3">
+      <c r="K154" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="155" spans="11:21" x14ac:dyDescent="0.3">
+      <c r="K155" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q155" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R155" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S155" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="156" spans="11:21" x14ac:dyDescent="0.3">
+      <c r="K156" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="157" spans="11:21" x14ac:dyDescent="0.3">
+      <c r="K157" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="158" spans="11:21" x14ac:dyDescent="0.3">
+      <c r="K158" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L85:M96">
     <sortCondition ref="L85:L96"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="U133:V133"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>